<commit_message>
yield rerun w/o enforcing min exp yields
</commit_message>
<xml_diff>
--- a/application/output_max_withoutMP_min_default_kapp/compiled_results.xlsx
+++ b/application/output_max_withoutMP_min_default_kapp/compiled_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG30"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,26 +575,6 @@
           <t>RBA: yield</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>FBA: yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>RBA: yield on minimal media at 1.0% exp. growth</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>RBA: yield on minimal media at 0.0% exp. growth</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -616,25 +596,25 @@
         <v>76.09</v>
       </c>
       <c r="E2" t="n">
-        <v>17.81382211868563</v>
+        <v>17.81382212023962</v>
       </c>
       <c r="F2" t="n">
-        <v>0.569551693020389</v>
+        <v>0.5695516930700739</v>
       </c>
       <c r="G2" t="n">
         <v>-13.21</v>
       </c>
       <c r="H2" t="n">
-        <v>7.603274750982186</v>
+        <v>7.603274750981975</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2430953884050908</v>
+        <v>0.243095388405084</v>
       </c>
       <c r="J2" t="n">
         <v>-13.21</v>
       </c>
       <c r="K2" t="n">
-        <v>0.426818832046538</v>
+        <v>0.4268188320092925</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -660,16 +640,12 @@
       </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="n">
-        <v>7.603274750982186</v>
+        <v>7.603274750981975</v>
       </c>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="n">
-        <v>0.2430953884050908</v>
-      </c>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
+        <v>0.243095388405084</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -691,25 +667,25 @@
         <v>122.16</v>
       </c>
       <c r="E3" t="n">
-        <v>2.555301938109797</v>
+        <v>2.555301936214222</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3122195099690078</v>
+        <v>0.3122195089297514</v>
       </c>
       <c r="G3" t="n">
-        <v>-5.549610203628807</v>
+        <v>-5.549610217984472</v>
       </c>
       <c r="H3" t="n">
-        <v>1.677292248506137</v>
+        <v>1.677284484134693</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08609664251008942</v>
+        <v>0.08609624395920293</v>
       </c>
       <c r="J3" t="n">
         <v>-13.21</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2757567665090363</v>
+        <v>0.2757554909183281</v>
       </c>
       <c r="L3" t="n">
         <v>0.08</v>
@@ -737,16 +713,12 @@
       </c>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="n">
-        <v>1.677292248506137</v>
+        <v>1.677284484134693</v>
       </c>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="n">
-        <v>0.08609664251008942</v>
-      </c>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
+        <v>0.08609624395920293</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -776,18 +748,10 @@
       <c r="G4" t="n">
         <v>-5.545419566892341</v>
       </c>
-      <c r="H4" t="n">
-        <v>2.782384540012428</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1053159090552506</v>
-      </c>
-      <c r="J4" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1582689694547692</v>
-      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
         <v>0.13</v>
       </c>
@@ -799,31 +763,15 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
-      <c r="W4" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
-        <v>2.782384540012428</v>
-      </c>
+      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="n">
-        <v>0.1053159090552506</v>
-      </c>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -853,18 +801,10 @@
       <c r="G5" t="n">
         <v>-5.544759808667549</v>
       </c>
-      <c r="H5" t="n">
-        <v>1.980862282753756</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.07497752701736145</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.1002437533622743</v>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>0.14</v>
       </c>
@@ -876,31 +816,15 @@
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
-      <c r="W5" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="n">
-        <v>1.980862282753756</v>
-      </c>
+      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="n">
-        <v>0.07497752701736145</v>
-      </c>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -930,18 +854,10 @@
       <c r="G6" t="n">
         <v>-5.545419566892341</v>
       </c>
-      <c r="H6" t="n">
-        <v>2.782384540012428</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.1053159090552506</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.1582689694547692</v>
-      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
         <v>0.13</v>
       </c>
@@ -953,31 +869,15 @@
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
-      <c r="W6" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="n">
-        <v>2.782384540012428</v>
-      </c>
+      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="n">
-        <v>0.1053159090552506</v>
-      </c>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1007,18 +907,10 @@
       <c r="G7" t="n">
         <v>-5.544759808667549</v>
       </c>
-      <c r="H7" t="n">
-        <v>1.980862282753756</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.07497752701736145</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.1002437533622743</v>
-      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>0.14</v>
       </c>
@@ -1030,31 +922,15 @@
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
-      <c r="W7" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="n">
-        <v>1.980862282753756</v>
-      </c>
+      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="n">
-        <v>0.07497752701736145</v>
-      </c>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1085,16 +961,16 @@
         <v>-5.549441423005486</v>
       </c>
       <c r="H8" t="n">
-        <v>1.508393595748058</v>
+        <v>1.508393595734358</v>
       </c>
       <c r="I8" t="n">
-        <v>0.08690249841046005</v>
+        <v>0.08690249840967075</v>
       </c>
       <c r="J8" t="n">
         <v>-13.21</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1888877319150266</v>
+        <v>0.188887731913311</v>
       </c>
       <c r="L8" t="n">
         <v>0.07000000000000001</v>
@@ -1122,16 +998,12 @@
       </c>
       <c r="Z8" t="inlineStr"/>
       <c r="AA8" t="n">
-        <v>1.508393595748058</v>
+        <v>1.508393595734358</v>
       </c>
       <c r="AB8" t="inlineStr"/>
       <c r="AC8" t="n">
-        <v>0.08690249841046005</v>
-      </c>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
+        <v>0.08690249840967075</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1153,25 +1025,25 @@
         <v>234.33</v>
       </c>
       <c r="E9" t="n">
-        <v>2.844697655376329</v>
+        <v>2.844697659175361</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2800995809453723</v>
+        <v>0.2800995813194391</v>
       </c>
       <c r="G9" t="n">
         <v>-13.21</v>
       </c>
       <c r="H9" t="n">
-        <v>0.303006696869241</v>
+        <v>0.303006696975616</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0298351737508245</v>
+        <v>0.02983517376129858</v>
       </c>
       <c r="J9" t="n">
         <v>-13.21</v>
       </c>
       <c r="K9" t="n">
-        <v>0.1065163098428314</v>
+        <v>0.1065163097379753</v>
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -1197,16 +1069,12 @@
       </c>
       <c r="Z9" t="inlineStr"/>
       <c r="AA9" t="n">
-        <v>0.303006696869241</v>
+        <v>0.303006696975616</v>
       </c>
       <c r="AB9" t="inlineStr"/>
       <c r="AC9" t="n">
-        <v>0.0298351737508245</v>
-      </c>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
+        <v>0.02983517376129858</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1237,16 +1105,16 @@
         <v>-5.547686668594033</v>
       </c>
       <c r="H10" t="n">
-        <v>4.964587466408677</v>
+        <v>4.964587119160285</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1879978148270952</v>
+        <v>0.1879978016775758</v>
       </c>
       <c r="J10" t="n">
         <v>-13.21</v>
       </c>
       <c r="K10" t="n">
-        <v>0.416259797319335</v>
+        <v>0.4162597682040166</v>
       </c>
       <c r="L10" t="n">
         <v>0.11</v>
@@ -1274,16 +1142,12 @@
       </c>
       <c r="Z10" t="inlineStr"/>
       <c r="AA10" t="n">
-        <v>4.964587466408677</v>
+        <v>4.964587119160285</v>
       </c>
       <c r="AB10" t="inlineStr"/>
       <c r="AC10" t="n">
-        <v>0.1879978148270952</v>
-      </c>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
+        <v>0.1879978016775758</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1305,25 +1169,25 @@
         <v>74.12</v>
       </c>
       <c r="E11" t="n">
-        <v>4.161856555785725</v>
+        <v>4.161856555785747</v>
       </c>
       <c r="F11" t="n">
-        <v>0.308528169914302</v>
+        <v>0.3085281699143037</v>
       </c>
       <c r="G11" t="n">
         <v>-5.549820853803197</v>
       </c>
       <c r="H11" t="n">
-        <v>1.643145652115875</v>
+        <v>1.643125404324842</v>
       </c>
       <c r="I11" t="n">
-        <v>0.05117524427556369</v>
+        <v>0.0511746136646067</v>
       </c>
       <c r="J11" t="n">
         <v>-13.21</v>
       </c>
       <c r="K11" t="n">
-        <v>0.1658689522249405</v>
+        <v>0.1658669082917806</v>
       </c>
       <c r="L11" t="n">
         <v>0.04</v>
@@ -1351,16 +1215,12 @@
       </c>
       <c r="Z11" t="inlineStr"/>
       <c r="AA11" t="n">
-        <v>1.643145652115875</v>
+        <v>1.643125404324842</v>
       </c>
       <c r="AB11" t="inlineStr"/>
       <c r="AC11" t="n">
-        <v>0.05117524427556369</v>
-      </c>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
+        <v>0.0511746136646067</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1385,22 +1245,22 @@
         <v>12.48937108880216</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7667243171293747</v>
+        <v>0.7667243171293748</v>
       </c>
       <c r="G12" t="n">
         <v>-13.21</v>
       </c>
       <c r="H12" t="n">
-        <v>1.484989845023696</v>
+        <v>1.484989845155429</v>
       </c>
       <c r="I12" t="n">
-        <v>0.09116374369648499</v>
+        <v>0.0911637437045721</v>
       </c>
       <c r="J12" t="n">
         <v>-13.21</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1189002900518444</v>
+        <v>0.118900290062392</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -1426,16 +1286,12 @@
       </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
-        <v>1.484989845023696</v>
+        <v>1.484989845155429</v>
       </c>
       <c r="AB12" t="inlineStr"/>
       <c r="AC12" t="n">
-        <v>0.09116374369648499</v>
-      </c>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
+        <v>0.0911637437045721</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1465,18 +1321,10 @@
       <c r="G13" t="n">
         <v>-5.548570274707247</v>
       </c>
-      <c r="H13" t="n">
-        <v>1.253882440223427</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.08595919709288039</v>
-      </c>
-      <c r="J13" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.2016467360444609</v>
-      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>0.15</v>
       </c>
@@ -1488,31 +1336,15 @@
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
-      <c r="W13" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="n">
-        <v>1.253882440223427</v>
-      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="n">
-        <v>0.08595919709288039</v>
-      </c>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1534,26 +1366,18 @@
         <v>256.4</v>
       </c>
       <c r="E14" t="n">
-        <v>1.016994536421403</v>
+        <v>1.016994536421399</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2607839207207038</v>
+        <v>0.2607839207207027</v>
       </c>
       <c r="G14" t="n">
-        <v>-5.550180402242264</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.370652195996508</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0.03993310224313486</v>
-      </c>
-      <c r="J14" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0.1531271641778202</v>
-      </c>
+        <v>-5.550180402242267</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
         <v>0.1</v>
       </c>
@@ -1565,31 +1389,15 @@
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
-      <c r="W14" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="n">
-        <v>0.370652195996508</v>
-      </c>
+      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="n">
-        <v>0.03993310224313486</v>
-      </c>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1611,25 +1419,25 @@
         <v>242.44</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9874314782806415</v>
+        <v>0.9874314721363102</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2393940695205564</v>
+        <v>0.239394068030912</v>
       </c>
       <c r="G15" t="n">
-        <v>-5.550717505065707</v>
+        <v>-5.55071750506583</v>
       </c>
       <c r="H15" t="n">
-        <v>0.400442259543859</v>
+        <v>0.400445192664307</v>
       </c>
       <c r="I15" t="n">
-        <v>0.04079365609768412</v>
+        <v>0.04079395489908182</v>
       </c>
       <c r="J15" t="n">
         <v>-13.21</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1704037872758633</v>
+        <v>0.1704050364932779</v>
       </c>
       <c r="L15" t="n">
         <v>0.005</v>
@@ -1657,16 +1465,12 @@
       </c>
       <c r="Z15" t="inlineStr"/>
       <c r="AA15" t="n">
-        <v>0.400442259543859</v>
+        <v>0.400445192664307</v>
       </c>
       <c r="AB15" t="inlineStr"/>
       <c r="AC15" t="n">
-        <v>0.04079365609768412</v>
-      </c>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr"/>
+        <v>0.04079395489908182</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1696,18 +1500,10 @@
       <c r="G16" t="n">
         <v>-5.549184128068436</v>
       </c>
-      <c r="H16" t="n">
-        <v>1.203868573870632</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0.03749410057725026</v>
-      </c>
-      <c r="J16" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.1079109946566728</v>
-      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
         <v>0.06</v>
       </c>
@@ -1719,31 +1515,15 @@
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
-      <c r="W16" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="n">
-        <v>1.203868573870632</v>
-      </c>
+      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>0.03749410057725026</v>
-      </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1773,18 +1553,10 @@
       <c r="G17" t="n">
         <v>-5.516810175715775</v>
       </c>
-      <c r="H17" t="n">
-        <v>14.73768830499428</v>
-      </c>
-      <c r="I17" t="n">
-        <v>0.5515809661594826</v>
-      </c>
-      <c r="J17" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.6946571304851238</v>
-      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="n">
         <v>0.6899999999999999</v>
       </c>
@@ -1796,31 +1568,15 @@
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
-      <c r="W17" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="n">
-        <v>14.73768830499428</v>
-      </c>
+      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="n">
-        <v>0.5515809661594826</v>
-      </c>
-      <c r="AD17" t="inlineStr"/>
-      <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
-      <c r="AG17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1842,25 +1598,25 @@
         <v>140.09</v>
       </c>
       <c r="E18" t="n">
-        <v>3.836460770451315</v>
+        <v>3.836460797193417</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5375941614562846</v>
+        <v>0.5375941652045984</v>
       </c>
       <c r="G18" t="n">
-        <v>-5.549254244910345</v>
+        <v>-5.549254244899956</v>
       </c>
       <c r="H18" t="n">
-        <v>1.686107340195298</v>
+        <v>1.686107340195276</v>
       </c>
       <c r="I18" t="n">
-        <v>0.09925235175857905</v>
+        <v>0.09925235175857776</v>
       </c>
       <c r="J18" t="n">
         <v>-13.21</v>
       </c>
       <c r="K18" t="n">
-        <v>0.1846231951063515</v>
+        <v>0.184623193819085</v>
       </c>
       <c r="L18" t="n">
         <v>0.07000000000000001</v>
@@ -1888,16 +1644,12 @@
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="n">
-        <v>1.686107340195298</v>
+        <v>1.686107340195276</v>
       </c>
       <c r="AB18" t="inlineStr"/>
       <c r="AC18" t="n">
-        <v>0.09925235175857905</v>
-      </c>
-      <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="inlineStr"/>
-      <c r="AF18" t="inlineStr"/>
-      <c r="AG18" t="inlineStr"/>
+        <v>0.09925235175857776</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1919,25 +1671,25 @@
         <v>272.25</v>
       </c>
       <c r="E19" t="n">
-        <v>3.969093042076502</v>
+        <v>3.969093036182585</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4540541189919563</v>
+        <v>0.4540541183177073</v>
       </c>
       <c r="G19" t="n">
         <v>-13.21</v>
       </c>
       <c r="H19" t="n">
-        <v>0.400094572882544</v>
+        <v>0.400094572886362</v>
       </c>
       <c r="I19" t="n">
-        <v>0.04576979851009124</v>
+        <v>0.04576979851052801</v>
       </c>
       <c r="J19" t="n">
         <v>-13.21</v>
       </c>
       <c r="K19" t="n">
-        <v>0.1008025180163646</v>
+        <v>0.1008025181670135</v>
       </c>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
@@ -1963,16 +1715,12 @@
       </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="n">
-        <v>0.400094572882544</v>
+        <v>0.400094572886362</v>
       </c>
       <c r="AB19" t="inlineStr"/>
       <c r="AC19" t="n">
-        <v>0.04576979851009124</v>
-      </c>
-      <c r="AD19" t="inlineStr"/>
-      <c r="AE19" t="inlineStr"/>
-      <c r="AF19" t="inlineStr"/>
-      <c r="AG19" t="inlineStr"/>
+        <v>0.04576979851052801</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2002,18 +1750,10 @@
       <c r="G20" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H20" t="n">
-        <v>0.100790276286722</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.2374729155094452</v>
-      </c>
-      <c r="J20" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1.008269369463034</v>
-      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
@@ -2043,35 +1783,15 @@
         </is>
       </c>
       <c r="T20" t="inlineStr"/>
-      <c r="U20" t="n">
-        <v>0.135358218584754</v>
-      </c>
+      <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
-      <c r="W20" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="n">
-        <v>0.100790276286722</v>
-      </c>
+      <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="n">
-        <v>0.2374729155094452</v>
-      </c>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="n">
-        <v>0.135743300793755</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0.078150819418957</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>0.08307504798705299</v>
-      </c>
+      <c r="AC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2093,26 +1813,18 @@
         <v>242.44</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1141673830273941</v>
+        <v>0.1141673830273931</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2428832021681819</v>
+        <v>0.2428832021681798</v>
       </c>
       <c r="G21" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H21" t="n">
-        <v>0.115079869491406</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.2448244539376226</v>
-      </c>
-      <c r="J21" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K21" t="n">
-        <v>1.007992532015847</v>
-      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
@@ -2138,35 +1850,15 @@
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
-      <c r="U21" t="n">
-        <v>0.148477553061659</v>
-      </c>
+      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="n">
-        <v>0.115079869491406</v>
-      </c>
+      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="n">
-        <v>0.2448244539376226</v>
-      </c>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="n">
-        <v>0.148839083264092</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0.079358646518538</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>0.084589254540941</v>
-      </c>
+      <c r="AC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2188,26 +1880,18 @@
         <v>103.1</v>
       </c>
       <c r="E22" t="n">
-        <v>4.826633115573244</v>
+        <v>4.826633115573516</v>
       </c>
       <c r="F22" t="n">
-        <v>0.4979383117364437</v>
+        <v>0.497938311736471</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.547262026771106</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1.443972089041542</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.06255555992283472</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-13.21</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0.1256291360764887</v>
-      </c>
+        <v>-5.547262026771114</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
         <v>0.13</v>
       </c>
@@ -2219,31 +1903,15 @@
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
-      <c r="W22" t="n">
-        <v>-13.21</v>
-      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="n">
-        <v>1.443972089041542</v>
-      </c>
+      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="n">
-        <v>0.06255555992283472</v>
-      </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="inlineStr"/>
-      <c r="AF22" t="inlineStr"/>
-      <c r="AG22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2274,16 +1942,16 @@
         <v>-13.21</v>
       </c>
       <c r="H23" t="n">
-        <v>0.203124484767071</v>
+        <v>0.203122931650805</v>
       </c>
       <c r="I23" t="n">
-        <v>0.02811475629451245</v>
+        <v>0.02811454132542408</v>
       </c>
       <c r="J23" t="n">
         <v>-13.21</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0808892261623313</v>
+        <v>0.08088860767277281</v>
       </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
@@ -2309,16 +1977,12 @@
       </c>
       <c r="Z23" t="inlineStr"/>
       <c r="AA23" t="n">
-        <v>0.203124484767071</v>
+        <v>0.203122931650805</v>
       </c>
       <c r="AB23" t="inlineStr"/>
       <c r="AC23" t="n">
-        <v>0.02811475629451245</v>
-      </c>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="inlineStr"/>
-      <c r="AF23" t="inlineStr"/>
-      <c r="AG23" t="inlineStr"/>
+        <v>0.02811454132542408</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2340,25 +2004,25 @@
         <v>228.24</v>
       </c>
       <c r="E24" t="n">
-        <v>1.465955759336204</v>
+        <v>1.465955758988919</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3345898406096754</v>
+        <v>0.3345898405304117</v>
       </c>
       <c r="G24" t="n">
-        <v>-5.550743282537632</v>
+        <v>-5.550743282537622</v>
       </c>
       <c r="H24" t="n">
-        <v>0.400094572755717</v>
+        <v>0.40009457288279</v>
       </c>
       <c r="I24" t="n">
-        <v>0.03837097817679252</v>
+        <v>0.03837097818897942</v>
       </c>
       <c r="J24" t="n">
         <v>-13.21</v>
       </c>
       <c r="K24" t="n">
-        <v>0.1146806433419334</v>
+        <v>0.1146806434055244</v>
       </c>
       <c r="L24" t="n">
         <v>0.0002</v>
@@ -2386,16 +2050,12 @@
       </c>
       <c r="Z24" t="inlineStr"/>
       <c r="AA24" t="n">
-        <v>0.400094572755717</v>
+        <v>0.40009457288279</v>
       </c>
       <c r="AB24" t="inlineStr"/>
       <c r="AC24" t="n">
-        <v>0.03837097817679252</v>
-      </c>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="inlineStr"/>
-      <c r="AF24" t="inlineStr"/>
-      <c r="AG24" t="inlineStr"/>
+        <v>0.03837097818897942</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2426,16 +2086,16 @@
         <v>-5.550726324289684</v>
       </c>
       <c r="H25" t="n">
-        <v>0.273747905701509</v>
+        <v>0.273747905701475</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02833111512552594</v>
+        <v>0.02833111512552243</v>
       </c>
       <c r="J25" t="n">
         <v>-13.21</v>
       </c>
       <c r="K25" t="n">
-        <v>0.1030604268002173</v>
+        <v>0.1030604268002045</v>
       </c>
       <c r="L25" t="n">
         <v>0.003</v>
@@ -2463,16 +2123,12 @@
       </c>
       <c r="Z25" t="inlineStr"/>
       <c r="AA25" t="n">
-        <v>0.273747905701509</v>
+        <v>0.273747905701475</v>
       </c>
       <c r="AB25" t="inlineStr"/>
       <c r="AC25" t="n">
-        <v>0.02833111512552594</v>
-      </c>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="inlineStr"/>
-      <c r="AF25" t="inlineStr"/>
-      <c r="AG25" t="inlineStr"/>
+        <v>0.02833111512552243</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2503,16 +2159,16 @@
         <v>-13.21</v>
       </c>
       <c r="H26" t="n">
-        <v>1.894526122141673</v>
+        <v>1.894526122141629</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1386348855850593</v>
+        <v>0.1386348855850561</v>
       </c>
       <c r="J26" t="n">
         <v>-13.21</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1947968203719789</v>
+        <v>0.1947968203719743</v>
       </c>
       <c r="L26" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
@@ -2538,16 +2194,12 @@
       </c>
       <c r="Z26" t="inlineStr"/>
       <c r="AA26" t="n">
-        <v>1.894526122141673</v>
+        <v>1.894526122141629</v>
       </c>
       <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
-        <v>0.1386348855850593</v>
-      </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="inlineStr"/>
-      <c r="AF26" t="inlineStr"/>
-      <c r="AG26" t="inlineStr"/>
+        <v>0.1386348855850561</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2577,18 +2229,10 @@
       <c r="G27" t="n">
         <v>-0.332925</v>
       </c>
-      <c r="H27" t="n">
-        <v>0.102247504860163</v>
-      </c>
-      <c r="I27" t="n">
-        <v>0.2427007657977054</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-0.332925</v>
-      </c>
-      <c r="K27" t="n">
-        <v>1.008401907812974</v>
-      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr">
@@ -2614,35 +2258,15 @@
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
-      <c r="U27" t="n">
-        <v>0.15276519020913</v>
-      </c>
+      <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
-      <c r="W27" t="n">
-        <v>-0.332925</v>
-      </c>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="n">
-        <v>0.102247504860163</v>
-      </c>
+      <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="n">
-        <v>0.2427007657977054</v>
-      </c>
-      <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="n">
-        <v>0.153175639705909</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0.078807086651177</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>0.08371505342808699</v>
-      </c>
+      <c r="AC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2664,25 +2288,25 @@
         <v>104.15</v>
       </c>
       <c r="E28" t="n">
-        <v>2.491549779661391</v>
+        <v>2.491549779661275</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2594955560978293</v>
+        <v>0.2594955560978174</v>
       </c>
       <c r="G28" t="n">
-        <v>-5.550731080009665</v>
+        <v>-5.550731080009659</v>
       </c>
       <c r="H28" t="n">
-        <v>1.36817810576082</v>
+        <v>1.368178106242954</v>
       </c>
       <c r="I28" t="n">
-        <v>0.05987566672387565</v>
+        <v>0.05987566674497531</v>
       </c>
       <c r="J28" t="n">
         <v>-13.21</v>
       </c>
       <c r="K28" t="n">
-        <v>0.230738697896247</v>
+        <v>0.2307386979775679</v>
       </c>
       <c r="L28" t="n">
         <v>0.001</v>
@@ -2710,16 +2334,12 @@
       </c>
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="n">
-        <v>1.36817810576082</v>
+        <v>1.368178106242954</v>
       </c>
       <c r="AB28" t="inlineStr"/>
       <c r="AC28" t="n">
-        <v>0.05987566672387565</v>
-      </c>
-      <c r="AD28" t="inlineStr"/>
-      <c r="AE28" t="inlineStr"/>
-      <c r="AF28" t="inlineStr"/>
-      <c r="AG28" t="inlineStr"/>
+        <v>0.05987566674497531</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2741,26 +2361,18 @@
         <v>824.3</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1308423337395128</v>
+        <v>0.1308423257890916</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2719810911745942</v>
+        <v>0.2719810746481062</v>
       </c>
       <c r="G29" t="n">
         <v>-2.20113372715757</v>
       </c>
-      <c r="H29" t="n">
-        <v>0.010665980963197</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0.02217130387320291</v>
-      </c>
-      <c r="J29" t="n">
-        <v>-2.201133727157571</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0.08151781352686159</v>
-      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
       <c r="L29" t="n">
         <v>0.14</v>
       </c>
@@ -2784,31 +2396,15 @@
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>UNDF</t>
-        </is>
-      </c>
+      <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
-      <c r="W29" t="n">
-        <v>-2.201133727157571</v>
-      </c>
+      <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="n">
-        <v>0.010665980963197</v>
-      </c>
+      <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr"/>
-      <c r="AC29" t="n">
-        <v>0.02217130387320291</v>
-      </c>
-      <c r="AD29" t="inlineStr"/>
-      <c r="AE29" t="inlineStr"/>
-      <c r="AF29" t="inlineStr"/>
-      <c r="AG29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2876,10 +2472,6 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
       <c r="AC30" t="inlineStr"/>
-      <c r="AD30" t="inlineStr"/>
-      <c r="AE30" t="inlineStr"/>
-      <c r="AF30" t="inlineStr"/>
-      <c r="AG30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>